<commit_message>
Complete adherence scoring system with 100% test coverage
✅ Achievement: All 73 algorithm configurations pass comprehensive testing

Major Updates:
- Enhanced testing framework to handle all 6 algorithm types
- Fixed config naming issues (REC0015 series corrected)
- Added time string support for caffeine cutoff patterns
- Created comprehensive WellPath Adherence Scoring Implementation Guide

Technical Details:
- test_all_73.py: Systematic batch testing of all configurations
- test_complex_config_validation.py: Enhanced with full algorithm support
- Config renames: Fixed misnamed REC0015.* files (minimum_frequency/weekly_elimination)
- Time handling: Added proper support for "14:00" style time thresholds

System Status:
- 73/73 configurations: ✅ PASS (100% success rate)
- 6 algorithm types: Fully implemented and tested
- Production ready: Complete testing coverage and documentation

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Scoring factors.xlsx
+++ b/Scoring factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c3d417d339670cb/Documents/GitHub/preliminary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{1BDF51E7-5E11-4E99-AA4A-5DD579AE109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DF808A1-8405-4416-9869-AE88FD9BEB99}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{1BDF51E7-5E11-4E99-AA4A-5DD579AE109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B55A8F3-6318-44CF-AD70-64FBC2F9F53D}"/>
   <bookViews>
-    <workbookView xWindow="38310" yWindow="0" windowWidth="19380" windowHeight="20970" tabRatio="864" firstSheet="15" activeTab="21" xr2:uid="{7BAB5CB3-E514-4AC3-9A35-1DA93A51C3CB}"/>
+    <workbookView minimized="1" xWindow="38110" yWindow="1950" windowWidth="28800" windowHeight="15370" tabRatio="864" firstSheet="15" activeTab="21" xr2:uid="{7BAB5CB3-E514-4AC3-9A35-1DA93A51C3CB}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerQuery &gt;&gt;&gt;" sheetId="20" r:id="rId1"/>
@@ -2705,7 +2705,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2746,6 +2746,9 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -16547,10 +16550,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="O15:AA31"/>
+  <dimension ref="O15:AA35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30:U31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P13" workbookViewId="0">
+      <selection activeCell="U35" sqref="U35:U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16853,6 +16856,9 @@
     </row>
     <row r="31" spans="15:27" x14ac:dyDescent="0.25">
       <c r="U31" s="22"/>
+    </row>
+    <row r="35" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R35" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Complete WellPath adherence system documentation and testing cleanup
- Updated root README.md to comprehensively cover entire platform:
  * Phase 1: Patient generation with synthetic data
  * Phase 2: Health assessment pipeline (7-pillar scoring)
  * Phase 3: Adherence architecture (8 core algorithms, 73+ configs tested)
  * Phase 4: Future extensions (challenges & triggering system)
- Created WellPath-Adherence-System-Overview.md executive summary
- Renamed test_all_73.py → test_all.py (scalable for any number of configs)
- Deleted outdated test files referencing old 14-algorithm classification
- Maintained essential testing: test_all.py + test_complex_config_validation.py

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Scoring factors.xlsx
+++ b/Scoring factors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2c3d417d339670cb/Documents/GitHub/preliminary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="186" documentId="8_{1BDF51E7-5E11-4E99-AA4A-5DD579AE109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B55A8F3-6318-44CF-AD70-64FBC2F9F53D}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="8_{1BDF51E7-5E11-4E99-AA4A-5DD579AE109A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A89B638-F9F3-4A2D-BFF3-DE89998076C8}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="38110" yWindow="1950" windowWidth="28800" windowHeight="15370" tabRatio="864" firstSheet="15" activeTab="21" xr2:uid="{7BAB5CB3-E514-4AC3-9A35-1DA93A51C3CB}"/>
+    <workbookView xWindow="38310" yWindow="0" windowWidth="19380" windowHeight="20970" tabRatio="864" firstSheet="15" activeTab="21" xr2:uid="{7BAB5CB3-E514-4AC3-9A35-1DA93A51C3CB}"/>
   </bookViews>
   <sheets>
     <sheet name="PowerQuery &gt;&gt;&gt;" sheetId="20" r:id="rId1"/>
@@ -16550,10 +16550,10 @@
   <sheetPr>
     <tabColor theme="2" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="O15:AA35"/>
+  <dimension ref="O15:AA48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="P13" workbookViewId="0">
-      <selection activeCell="U35" sqref="U35:U42"/>
+      <selection activeCell="V49" sqref="V49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -16857,8 +16857,14 @@
     <row r="31" spans="15:27" x14ac:dyDescent="0.25">
       <c r="U31" s="22"/>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="18:22" x14ac:dyDescent="0.25">
       <c r="R35" s="23"/>
+    </row>
+    <row r="48" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="V48" s="21">
+        <f>323-73-112</f>
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>